<commit_message>
Adding the method to fetch new customer with phone number
</commit_message>
<xml_diff>
--- a/testData/Hana_T303.xlsx
+++ b/testData/Hana_T303.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD8085F-5108-4400-B26F-FB4B1596370D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7D5ECF-E90C-42C0-AB72-A9BA2B953524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="1200" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>custaddress1</t>
   </si>
   <si>
-    <t>2715 35th Ave</t>
-  </si>
-  <si>
     <t>custzip</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Cash Register2</t>
+  </si>
+  <si>
+    <t>2715 35th Avenue Greeley, CO, USA</t>
   </si>
 </sst>
 </file>
@@ -490,13 +490,13 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
@@ -522,10 +522,10 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -564,7 +564,7 @@
         <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -572,10 +572,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
@@ -614,10 +614,10 @@
         <v>0</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>